<commit_message>
pictures music and videos update + stuffs
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1602670361" val="978" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1602670361" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1602670361"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1602670361"/>
+      <pm:revision xmlns:pm="smNativeData" day="1602768807" val="978" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1602768807" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1602768807" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1602768807"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Added music</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>own's music and moshi moshi album</t>
+  </si>
+  <si>
+    <t>work on navi bar</t>
   </si>
   <si>
     <t>Page redesign</t>
@@ -80,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;¥&quot;;\-#,##0\ &quot;¥&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;¥&quot;;[Red]\-#,##0\ &quot;¥&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;¥&quot;;\-#,##0.00\ &quot;¥&quot;"/>
@@ -89,8 +92,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _¥_-;\-* #,##0\ _¥_-;_-* &quot;-&quot;\ _¥_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;¥&quot;_-;\-* #,##0.00\ &quot;¥&quot;_-;_-* &quot;-&quot;??\ &quot;¥&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _¥_-;\-* #,##0.00\ _¥_-;_-* &quot;-&quot;??\ _¥_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD;@"/>
+    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -100,7 +102,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1602670361" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1602768807" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -122,7 +124,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1602670361" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1602768807" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -144,7 +146,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1602670361"/>
+          <pm:border xmlns:pm="smNativeData" id="1602768807"/>
         </ext>
       </extLst>
     </border>
@@ -163,7 +165,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1602670361"/>
+          <pm:border xmlns:pm="smNativeData" id="1602768807"/>
         </ext>
       </extLst>
     </border>
@@ -171,15 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -189,7 +188,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1602670361" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1602768807" count="1">
         <pm:charStyle name="標準" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -453,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A4:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -469,7 +468,7 @@
     <col min="6" max="6" width="49.729730" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="n">
         <v>44118</v>
       </c>
@@ -481,6 +480,9 @@
       </c>
       <c r="D4" t="s">
         <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -488,13 +490,13 @@
         <v>44118</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -502,10 +504,13 @@
         <v>44120</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -513,22 +518,22 @@
         <v>44123</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="2" t="n">
         <v>44125</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -536,10 +541,10 @@
         <v>44127</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -547,10 +552,10 @@
         <v>44128</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -558,17 +563,17 @@
         <v>44131</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1602670361" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1602768807" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -577,16 +582,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1602670361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1602670361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1602670361" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1602670361" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1602768807" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1602768807" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1602768807" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1602768807" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1602670361" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1602768807" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
changed htmls in js
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1602940205" val="978" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1602940205" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1602940205" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1602940205"/>
+      <pm:revision xmlns:pm="smNativeData" day="1603633657" val="978" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1603633657" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1603633657" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1603633657"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Added music</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>set up the templates and elements</t>
+  </si>
+  <si>
+    <t>multiple buttons for multiple sizes for manga</t>
   </si>
   <si>
     <t>lewd collection</t>
@@ -123,7 +126,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1602940205" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1603633657" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -132,7 +135,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,13 +148,68 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1602940205" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1603633657" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3DFF3D"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1603633657" type="1" fgLvl="76" fgClr="0000FF00" bgLvl="24" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1603633657" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1603633657" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF3D"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1603633657" type="1" fgLvl="76" fgClr="00FFFF00" bgLvl="24" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9E9E"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1603633657" type="1" fgLvl="38" fgClr="00FF0000" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -167,7 +225,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1602940205"/>
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
         </ext>
       </extLst>
     </border>
@@ -186,7 +244,102 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1602940205"/>
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1603633657"/>
         </ext>
       </extLst>
     </border>
@@ -194,12 +347,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -209,7 +390,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1602940205" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1603633657" count="1">
         <pm:charStyle name="標準" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -476,7 +657,7 @@
   <dimension ref="A4:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -489,149 +670,163 @@
     <col min="6" max="6" width="49.729730" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:7" s="3" customFormat="1">
+      <c r="A4" s="4" t="n">
         <v>44118</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:6" s="3" customFormat="1">
+      <c r="A5" s="4" t="n">
         <v>44118</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="6:6">
-      <c r="F6" t="s">
+    <row r="6" spans="1:6" s="3" customFormat="1">
+      <c r="A6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:6" s="3" customFormat="1">
+      <c r="A7" s="4" t="n">
         <v>44120</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="n">
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1">
+      <c r="A8" s="4"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1">
+      <c r="A9" s="4" t="n">
         <v>44123</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="n">
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1">
+      <c r="A10" s="4" t="n">
         <v>44123</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="n">
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="12" customFormat="1">
+      <c r="A11" s="13" t="n">
         <v>44125</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" t="s">
+      <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2" t="n">
+      <c r="E11" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="6" customFormat="1">
+      <c r="A12" s="7" t="n">
         <v>44127</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="n">
+    </row>
+    <row r="13" spans="1:4" s="6" customFormat="1">
+      <c r="A13" s="7" t="n">
         <v>44128</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="n">
+      <c r="C13" s="8"/>
+      <c r="D13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="9" customFormat="1">
+      <c r="A14" s="10" t="n">
         <v>44131</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="9" t="s">
         <v>24</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1602940205" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1603633657" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -640,16 +835,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1602940205" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1602940205" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1602940205" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1602940205" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1603633657" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1603633657" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1603633657" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1603633657" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1602940205" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1603633657" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>